<commit_message>
Modelo conceptual e Lógico
</commit_message>
<xml_diff>
--- a/LevantamentoRequisitos.xlsx
+++ b/LevantamentoRequisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Desktop\Universidade\UMinho\LCC 3 ano\1º Semestre\BD\TrabalhoPratico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F272CC-8EE8-4F63-9073-2A924330BB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AE14EB-3335-433D-AC1C-7F51F9C6480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{921132CD-A3A8-F74A-9E0F-4C9A16FC001E}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>RD06</t>
   </si>
   <si>
-    <t>Cada pedido deve conter o seu número de pedido, informações dos items e da sua entrega, endereço de entrega, data do pedido/envio/entrega, cliente associado,</t>
-  </si>
-  <si>
     <t>O cliente deve ser sempre notificado da alteração de um estado do pedido que fez</t>
   </si>
   <si>
@@ -200,10 +197,13 @@
     <t>Cada funcionário possui um id, nome, tipo, salário, endereço, armazém e desempenho.</t>
   </si>
   <si>
-    <t>Cada armazém tem um id, nome, conjunto de funcionários e items.</t>
-  </si>
-  <si>
     <t>Deve ser possível adicionar novos armazéns, funcionários, clientes e pedidos.</t>
+  </si>
+  <si>
+    <t>Cada pedido deve conter o seu número de pedido, endereço de entrega, data do pedido/envio/entrega, cliente associado,</t>
+  </si>
+  <si>
+    <t>Cada armazém tem um id, nome, localidade, conjunto de funcionários e items.</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A2:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -693,10 +693,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -712,13 +712,13 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
         <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -726,13 +726,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -740,13 +740,13 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -754,10 +754,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
@@ -768,13 +768,13 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
         <v>35</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -782,13 +782,13 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
         <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -796,10 +796,10 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
         <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
       </c>
       <c r="E18" t="s">
         <v>22</v>
@@ -810,13 +810,13 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
         <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -824,10 +824,10 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
         <v>23</v>
@@ -838,10 +838,10 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
         <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
@@ -852,13 +852,13 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
@@ -866,13 +866,13 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
@@ -880,10 +880,10 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
@@ -894,7 +894,7 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
@@ -902,7 +902,7 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Realmnete adicionand dessa vez
</commit_message>
<xml_diff>
--- a/LevantamentoRequisitos.xlsx
+++ b/LevantamentoRequisitos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
   <si>
     <t xml:space="preserve">Gestão de Análises Clinicas</t>
   </si>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">RD05</t>
   </si>
   <si>
-    <t xml:space="preserve">Os administrativos podem atualizar o sálario dos funcionários, alterar o estado dos pedidos e adicionar novos items.</t>
+    <t xml:space="preserve">Os administrativos podem atualizar o sálario dos funcionários, alterar o estado dos pedidos e adicionar e alterar itens.</t>
   </si>
   <si>
     <t xml:space="preserve">RC05</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">RC06</t>
   </si>
   <si>
-    <t xml:space="preserve">A cada pedido está associado um distribuidor e a cada distribuidor muitos pedidos.</t>
+    <t xml:space="preserve">A cada pedido estão associados varios funcionários e a cada funcionario muitos pedidos.</t>
   </si>
   <si>
     <t xml:space="preserve">RD06</t>
@@ -161,6 +161,114 @@
   </si>
   <si>
     <t xml:space="preserve">Deve ser possível adicionar novos armazéns, funcionários, clientes e pedidos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somente Jefferson Bazos tem controle sobre a informação completa da base de dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somente Jefferson bazos pode ter acessso a informação em relação aos gestores dos armazens </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somente o gestor do armazém e Jefferson bazos pode acessar os dados do seu armazem (funcionarios, itens , pedidos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obter o número de clientes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar o número de funcionários </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saber para cada pedido quais funcionarios estão associados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedidos/Funcionários</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conhecer o armazém em que o pedido está relacionado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armazém/Pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificar os clientes com maiores gastos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consultar os pedidos feitos por um cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clientes/Pedidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consultar os funcionários com melhores desempenho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificar os items mais vendidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saber para cada funcionario quais pedidos estão associados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obter quais funcionários trabalham em dado armazem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obter quais tipos de items são mais populares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obter uma relação entre salário e desempenho de cada funcionarios por tipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os funcionarios relacionados a um pedido tem acesso a informação desse pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcionários/Pedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC10</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -441,13 +549,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F26"/>
+  <dimension ref="A2:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="138"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14"/>
@@ -713,6 +821,221 @@
       </c>
       <c r="C26" s="0" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +1060,7 @@
       <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.8"/>
   </cols>
@@ -745,7 +1068,7 @@
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="F1" s="5" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,7 +1094,7 @@
     </row>
     <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -785,7 +1108,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -794,10 +1117,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -822,10 +1145,10 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.7"/>
   </cols>
@@ -833,7 +1156,7 @@
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="E1" s="7" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +1182,7 @@
     </row>
     <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -873,7 +1196,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -882,10 +1205,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -913,7 +1236,7 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
   </cols>
@@ -921,7 +1244,7 @@
     <row r="1" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="F1" s="7" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +1270,7 @@
     </row>
     <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -961,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -970,10 +1293,10 @@
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reparar os requisitos e alterar a viabilidade :sunglasses:
</commit_message>
<xml_diff>
--- a/LevantamentoRequisitos.xlsx
+++ b/LevantamentoRequisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Desktop\Universidade\UMinho\LCC 3 ano\1º Semestre\BD\TrabalhoPratico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC0D22E-AD94-46E2-B5C0-B6C4654355F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AF72D0-B8A9-4FE0-AB18-BCECDD79C95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
   <si>
     <t>Gestão de Análises Clinicas</t>
   </si>
@@ -322,6 +322,12 @@
   </si>
   <si>
     <t>RC11</t>
+  </si>
+  <si>
+    <t>Exploracao - dizer como o vamos fazer ( total dos clientes pelo id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -423,18 +429,18 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F43"/>
+  <dimension ref="A2:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -830,17 +836,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -851,7 +857,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
@@ -859,20 +865,20 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10">
@@ -1339,6 +1345,14 @@
       </c>
       <c r="E43" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1361,23 +1375,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="A1" s="6"/>
-      <c r="F1" s="7" t="s">
+      <c r="A1" s="4"/>
+      <c r="F1" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -1388,33 +1402,33 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1441,23 +1455,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="A1" s="6"/>
-      <c r="E1" s="8" t="s">
+      <c r="A1" s="4"/>
+      <c r="E1" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -1468,33 +1482,33 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1521,23 +1535,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="A1" s="6"/>
-      <c r="F1" s="8" t="s">
+      <c r="A1" s="4"/>
+      <c r="F1" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -1548,33 +1562,33 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>